<commit_message>
cambios en el servidor
</commit_message>
<xml_diff>
--- a/public/uploads/invitados.xlsx
+++ b/public/uploads/invitados.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto Santizo\Desktop\PROYECTOS\Boda Hermano Willy\Boda\public\uploads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB191E7-A3A5-4F45-9F00-41E35F31E6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="999999"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Nombre del Invitado</t>
   </si>
@@ -29,20 +24,39 @@
   </si>
   <si>
     <t>Felicitaciones</t>
+  </si>
+  <si>
+    <t>PRUEBA CEL</t>
+  </si>
+  <si>
+    <t>Novio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIEBA CEL 
+                    </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -90,22 +104,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -395,21 +401,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="9.140625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.7109375" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17.42578125" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +429,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ultimo cambios y agregacion de nuevo campo al formulario
</commit_message>
<xml_diff>
--- a/public/uploads/invitados.xlsx
+++ b/public/uploads/invitados.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto Santizo\Desktop\PROYECTOS\Boda Hermano Willy\Boda\public\uploads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8966A367-FD0E-4FB4-B0A5-CF358DE93C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Nombre del Invitado</t>
   </si>
@@ -26,37 +31,21 @@
     <t>Felicitaciones</t>
   </si>
   <si>
-    <t>PRUEBA CEL</t>
-  </si>
-  <si>
-    <t>Novio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIEBA CEL 
-                    </t>
+    <t>Número de Invitados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -104,14 +93,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,24 +398,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="9.140625" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13.7109375" customWidth="true" style="0"/>
-    <col min="3" max="3" width="17.42578125" customWidth="true" style="0"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" customHeight="1" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,23 +421,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
 </worksheet>
 </file>
</xml_diff>